<commit_message>
22.08.2025 18:58  коррекция excel
</commit_message>
<xml_diff>
--- a/crm2/data/schedule_2025_1_cohort.xlsx
+++ b/crm2/data/schedule_2025_1_cohort.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\PycharmProjects\ProjectCRM\crm2\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\PycharmProjects\crm\crm2\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{074F3556-21AE-49BA-A91A-83115633F1BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0061641-9B3F-4076-B941-9B4BBCB686B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A6D14E0E-4D6A-4D8A-BF55-A0F0A0859D24}"/>
   </bookViews>
@@ -86,9 +86,6 @@
     <t>17</t>
   </si>
   <si>
-    <t>Не-восприятие; 2.3. Работа с прото-формами, не-формами, смысловые практики; Формирование объемных фигур внимания; Превращение объекта внимания в фигуру внимания;Различение действия из ментальной тишины (МТ) и пауз; Работа с локальными объемами внимания;</t>
-  </si>
-  <si>
     <t>Остановка внимания; Остановка сознания;  Работа с Вниманием, ЛОВ; Циклы с ЛОВ; Работа с не-формами, не-восприятием</t>
   </si>
   <si>
@@ -114,6 +111,9 @@
   </si>
   <si>
     <t>Заключение</t>
+  </si>
+  <si>
+    <t>Не-восприятие; Работа с прото-формами, не-формами, смысловые практики; Формирование объемных фигур внимания; Превращение объекта внимания в фигуру внимания;Различение действия из ментальной тишины (МТ) и пауз; Работа с локальными объемами внимания;</t>
   </si>
 </sst>
 </file>
@@ -546,7 +546,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -592,10 +592,10 @@
         <v>7</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -612,10 +612,10 @@
         <v>8</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -632,10 +632,10 @@
         <v>9</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
@@ -652,10 +652,10 @@
         <v>10</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -672,10 +672,10 @@
         <v>6</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>